<commit_message>
Update input data file
</commit_message>
<xml_diff>
--- a/assignment_3/EPA1352-G13-A3/data/Overview_intersections.xlsx
+++ b/assignment_3/EPA1352-G13-A3/data/Overview_intersections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\epa1352advancedsimulation\assignment_3\EPA1352-G13-A3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F8B51-652A-4203-854F-FD437C59B38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A3D1DC-0895-46B9-806D-3783D688C0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>N210</t>
+  </si>
+  <si>
+    <t>Einde van de weg moet ook sourcesink zijn, want begin is ook. Start van de weg.</t>
+  </si>
+  <si>
+    <t>Staat er twee keer in</t>
+  </si>
+  <si>
+    <t>Zit er alleen in op N1, dus link van gemaakt.</t>
+  </si>
+  <si>
+    <t>Intersection 1686 heeft een conditie. 2512 ook. 325 ook.</t>
+  </si>
+  <si>
+    <t>3056 ook.</t>
   </si>
 </sst>
 </file>
@@ -93,7 +108,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -125,16 +146,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -415,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -482,27 +505,32 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="6">
         <v>1476</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>325</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>91.381360400000005</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>23.009555599999999</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="6"/>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -526,7 +554,7 @@
         <v>23.690416299999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="15.6" customHeight="1">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -536,7 +564,7 @@
       <c r="C6" s="1">
         <v>90.568804900000003</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>3.7851941</v>
       </c>
       <c r="E6" t="s">
@@ -550,7 +578,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="6">
         <v>1686</v>
       </c>
       <c r="E7" t="s">
@@ -603,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="H9">
-        <v>3279</v>
+        <v>3277</v>
       </c>
       <c r="I9" s="1">
         <v>91.510249999999999</v>
@@ -631,7 +659,7 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>3459</v>
       </c>
       <c r="I10" s="1">
@@ -658,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="H11">
-        <v>3019</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -678,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="H12">
-        <v>3056</v>
+        <v>3662</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -698,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="H13">
-        <v>3410</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -718,7 +746,45 @@
         <v>15</v>
       </c>
       <c r="H14">
-        <v>3655</v>
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2640</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>